<commit_message>
expenses report almost working
</commit_message>
<xml_diff>
--- a/Expenses2023-01-01-2023-02-09.xlsx
+++ b/Expenses2023-01-01-2023-02-09.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>PRODUCT SALES</t>
   </si>
@@ -36,6 +36,39 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>2023-02-08</t>
+  </si>
+  <si>
+    <t>Potatoes and Onions</t>
+  </si>
+  <si>
+    <t>Onions</t>
+  </si>
+  <si>
+    <t>Potatoes</t>
+  </si>
+  <si>
+    <t>Fries</t>
+  </si>
+  <si>
+    <t>Milk and Bread</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Eggs and Chicken</t>
+  </si>
+  <si>
+    <t>Beef, Onion and Potatoes</t>
+  </si>
+  <si>
+    <t>Ground Beef</t>
   </si>
 </sst>
 </file>
@@ -83,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:I4"/>
+  <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -120,6 +153,226 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="B5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G5" t="n" s="0">
+        <v>1.399999976158142</v>
+      </c>
+      <c r="H5" t="n" s="0">
+        <v>0.10000000149011612</v>
+      </c>
+      <c r="I5" s="0">
+        <f>D5*H5/F5*G5</f>
+      </c>
+    </row>
+    <row r="6">
+      <c r="E6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G6" t="n" s="0">
+        <v>1.7999999523162842</v>
+      </c>
+      <c r="H6" t="n" s="0">
+        <v>0.25</v>
+      </c>
+      <c r="I6" s="0">
+        <f>D5*H6/F6*G6</f>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8">
+      <c r="B8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G8" t="n" s="0">
+        <v>1.7999999523162842</v>
+      </c>
+      <c r="H8" t="n" s="0">
+        <v>0.25</v>
+      </c>
+      <c r="I8" s="0">
+        <f>D8*H8/F8*G8</f>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10">
+      <c r="B10" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="G10" t="n" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H10" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="I10" s="0">
+        <f>D10*H10/F10*G10</f>
+      </c>
+    </row>
+    <row r="11">
+      <c r="E11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G11" t="n" s="0">
+        <v>0.9900000095367432</v>
+      </c>
+      <c r="H11" t="n" s="0">
+        <v>0.4000000059604645</v>
+      </c>
+      <c r="I11" s="0">
+        <f>D10*H11/F11*G11</f>
+      </c>
+    </row>
+    <row r="12"/>
+    <row r="13">
+      <c r="B13" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F13" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="G13" t="n" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H13" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="I13" s="0">
+        <f>D13*H13/F13*G13</f>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G14" t="n" s="0">
+        <v>1.7999999523162842</v>
+      </c>
+      <c r="H14" t="n" s="0">
+        <v>0.3499999940395355</v>
+      </c>
+      <c r="I14" s="0">
+        <f>D13*H14/F14*G14</f>
+      </c>
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="B16" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F16" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G16" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="H16" t="n" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="0">
+        <f>D16*H16/F16*G16</f>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G17" t="n" s="0">
+        <v>1.399999976158142</v>
+      </c>
+      <c r="H17" t="n" s="0">
+        <v>0.15000000596046448</v>
+      </c>
+      <c r="I17" s="0">
+        <f>D16*H17/F17*G17</f>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F18" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G18" t="n" s="0">
+        <v>1.7999999523162842</v>
+      </c>
+      <c r="H18" t="n" s="0">
+        <v>0.6000000238418579</v>
+      </c>
+      <c r="I18" s="0">
+        <f>D16*H18/F18*G18</f>
+      </c>
+    </row>
+    <row r="19"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Expenses report working semi git push
</commit_message>
<xml_diff>
--- a/Expenses2023-01-01-2023-02-09.xlsx
+++ b/Expenses2023-01-01-2023-02-09.xlsx
@@ -128,7 +128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:J35"/>
+  <dimension ref="B2:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -576,6 +576,11 @@
         <f>SUM(J32:J34)</f>
       </c>
     </row>
+    <row r="37">
+      <c r="J37" s="2">
+        <f>SUM(J35,J30,J25,J21,J17,J14,J11,J7)</f>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
expenses report fully working
</commit_message>
<xml_diff>
--- a/Expenses2023-01-01-2023-02-09.xlsx
+++ b/Expenses2023-01-01-2023-02-09.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>PRODUCT SALES</t>
   </si>
@@ -72,16 +72,41 @@
   </si>
   <si>
     <t>Ground Beef</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Start Shift</t>
+  </si>
+  <si>
+    <t>End Shift</t>
+  </si>
+  <si>
+    <t>Total Hours</t>
+  </si>
+  <si>
+    <t>Salary/Hour</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(€* #,##0.00_);_(€* (#,##0.00);_(€* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(€* ###,##0.00_);_(€* (###,##0.00);_(€* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#####0.00"/>
+    <numFmt numFmtId="167" formatCode="HH:MM"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -117,18 +142,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:J37"/>
+  <dimension ref="B2:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -581,6 +607,37 @@
         <f>SUM(J35,J30,J25,J21,J17,J14,J11,J7)</f>
       </c>
     </row>
+    <row r="39">
+      <c r="B39" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F39" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G39" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H39" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="I39" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="I41" s="1">
+        <f>SUM(I41:I41)</f>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>